<commit_message>
8/9 Saving SheeData through streaming: Decrease memory usage during SheetData saving. Save SheetData by saving each row instead of creating whole DOM for all rows and saving everything in the the element at once. Test files had some empty rows (e.g. <x:row r="3" spans="1:6"/>) that were in the input file and originally was saved, but since they are invalid, they are now skipped.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotSubtotalsSource/input.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotSubtotalsSource/input.xlsx
@@ -1186,17 +1186,7 @@
     <x:col min="6" max="6" width="13.832031" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="3" spans="1:6"/>
     <x:row r="4" spans="1:6" ht="11.25" customHeight="1"/>
-    <x:row r="5" spans="1:6"/>
-    <x:row r="6" spans="1:6"/>
-    <x:row r="7" spans="1:6"/>
-    <x:row r="8" spans="1:6"/>
-    <x:row r="9" spans="1:6"/>
-    <x:row r="10" spans="1:6"/>
-    <x:row r="11" spans="1:6"/>
-    <x:row r="12" spans="1:6"/>
-    <x:row r="13" spans="1:6"/>
     <x:row r="14" spans="1:6" ht="12.75" customHeight="1"/>
     <x:row r="29" spans="1:6" ht="11.25" customHeight="1"/>
     <x:row r="30" spans="1:6" ht="11.25" customHeight="1"/>

</xml_diff>